<commit_message>
[ADD] PDF to project 4
</commit_message>
<xml_diff>
--- a/Mass_Table.xlsx
+++ b/Mass_Table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wutwaw-my.sharepoint.com/personal/01142427_pw_edu_pl/Documents/Dokumenty/Studia_magisterskie/UAV/UAV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D0573ACB-90EA-4FC4-9ACF-446431E0745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:40009_{D0573ACB-90EA-4FC4-9ACF-446431E0745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48B2AF7E-3FDF-4FD7-99E1-493AD47272C7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mass_Table" sheetId="1" r:id="rId1"/>
@@ -112,12 +112,6 @@
     <t>VN-310 DUALGNSS/INS</t>
   </si>
   <si>
-    <t>MTOW zał</t>
-  </si>
-  <si>
-    <t>MTOW realne</t>
-  </si>
-  <si>
     <t>Ixx</t>
   </si>
   <si>
@@ -128,13 +122,19 @@
   </si>
   <si>
     <t>S.C._Sca</t>
+  </si>
+  <si>
+    <t>MTOW założone</t>
+  </si>
+  <si>
+    <t>MTOW realne/ ostateczne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,8 +287,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -468,8 +475,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -584,6 +603,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -629,8 +663,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -985,32 +1022,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="42.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
@@ -1033,19 +1073,20 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>75</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>3.7</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
         <v>277.5</v>
       </c>
       <c r="I2">
@@ -1065,19 +1106,20 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>9.1</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1">
         <v>109.2</v>
       </c>
       <c r="I3">
@@ -1097,36 +1139,38 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>9.1</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
         <v>109.2</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>50</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>5.3</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
         <v>265</v>
       </c>
       <c r="I5">
@@ -1146,19 +1190,20 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>50</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>5.3</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
         <v>265</v>
       </c>
       <c r="I6">
@@ -1178,19 +1223,20 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>12.1</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
         <v>60.5</v>
       </c>
       <c r="I7">
@@ -1210,19 +1256,20 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>12.1</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
         <v>60.5</v>
       </c>
       <c r="I8">
@@ -1242,19 +1289,20 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>12.1</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
         <v>145.19999999999999</v>
       </c>
       <c r="I9">
@@ -1274,19 +1322,20 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>5.8</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
         <v>87</v>
       </c>
       <c r="I10">
@@ -1306,19 +1355,20 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>5.8</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
         <v>87</v>
       </c>
       <c r="I11">
@@ -1338,19 +1388,20 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>1.4</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
         <v>14</v>
       </c>
       <c r="I12">
@@ -1370,19 +1421,20 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>300</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>6.35</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
         <v>1905</v>
       </c>
       <c r="I13">
@@ -1402,19 +1454,20 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>15</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>6.5</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="F14">
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
         <v>97.5</v>
       </c>
       <c r="I14">
@@ -1434,19 +1487,20 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>10</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>1.5</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
         <v>15</v>
       </c>
       <c r="I15">
@@ -1466,19 +1520,20 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>50</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>2</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="F16">
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
         <v>100</v>
       </c>
       <c r="I16">
@@ -1498,16 +1553,18 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
         <v>0</v>
       </c>
       <c r="M17">
@@ -1515,16 +1572,18 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1">
         <v>0</v>
       </c>
       <c r="M18">
@@ -1532,19 +1591,20 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>220</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>5.34</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="F19">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
         <v>1175.57</v>
       </c>
       <c r="I19">
@@ -1564,10 +1624,14 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="F20">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1">
         <v>0</v>
       </c>
       <c r="I20">
@@ -1587,121 +1651,142 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>38</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>0.8</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="F21">
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
         <v>30.4</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>3.5</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>1.8</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="F22">
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
         <v>6.3</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>2.1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.5</v>
       </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="F23">
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
         <v>1.05</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.16</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>2</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="F24">
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1">
         <v>0.32</v>
       </c>
     </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+    </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1">
         <v>900</v>
       </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
       <c r="I26">
         <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1">
+        <v>899.8</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="1">
+        <v>4811</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B27">
-        <v>899.8</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B28" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F27">
-        <v>4811</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="F28" s="1">
+        <v>5.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28">
-        <v>0.87</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28">
-        <v>5.35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>